<commit_message>
LWOTimer, Knockback, PlayAnimation, PlayFXEffect, StopFXEffect, VE Stuff
</commit_message>
<xml_diff>
--- a/analysis/GameMessages.xlsx
+++ b/analysis/GameMessages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\LUReborn Server 3.0\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7041AC0F-4759-47E0-B1A4-3529B937DE7F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB87FE3E-19F1-4F8D-916B-42D9583C9335}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="1410" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="497">
   <si>
     <t>ID</t>
   </si>
@@ -1520,6 +1520,9 @@
   </si>
   <si>
     <t>HasSkill</t>
+  </si>
+  <si>
+    <t>TimerDone</t>
   </si>
 </sst>
 </file>
@@ -1527,7 +1530,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1581,7 +1584,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1870,8 +1873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1768"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A730" workbookViewId="0">
-      <selection activeCell="D737" sqref="D737"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="D306" sqref="D306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4863,7 +4866,7 @@
         <v>012F</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>304</v>
       </c>
@@ -4872,7 +4875,7 @@
         <v>0130</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>305</v>
       </c>
@@ -4880,8 +4883,14 @@
         <f t="shared" si="4"/>
         <v>0131</v>
       </c>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C306" t="s">
+        <v>496</v>
+      </c>
+      <c r="D306" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>306</v>
       </c>
@@ -4890,7 +4899,7 @@
         <v>0132</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>307</v>
       </c>
@@ -4899,7 +4908,7 @@
         <v>0133</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>308</v>
       </c>
@@ -4908,7 +4917,7 @@
         <v>0134</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>309</v>
       </c>
@@ -4917,7 +4926,7 @@
         <v>0135</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>310</v>
       </c>
@@ -4926,7 +4935,7 @@
         <v>0136</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>311</v>
       </c>
@@ -4935,7 +4944,7 @@
         <v>0137</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>312</v>
       </c>
@@ -4944,7 +4953,7 @@
         <v>0138</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>313</v>
       </c>
@@ -4953,7 +4962,7 @@
         <v>0139</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>314</v>
       </c>
@@ -4962,7 +4971,7 @@
         <v>013A</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>315</v>
       </c>
@@ -4971,7 +4980,7 @@
         <v>013B</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>316</v>
       </c>
@@ -4980,7 +4989,7 @@
         <v>013C</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>317</v>
       </c>
@@ -4989,7 +4998,7 @@
         <v>013D</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>318</v>
       </c>
@@ -4998,7 +5007,7 @@
         <v>013E</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>319</v>
       </c>
@@ -21007,7 +21016,7 @@
       </c>
       <c r="B4">
         <f>COUNTIF(Data!C:C,"&lt;&gt;")-1</f>
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -21016,7 +21025,7 @@
       </c>
       <c r="B5">
         <f>B3-B4</f>
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -21025,7 +21034,7 @@
       </c>
       <c r="B6" s="1">
         <f>1/B3*B4</f>
-        <v>0.32710809281267689</v>
+        <v>0.32767402376910021</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -21043,7 +21052,7 @@
       </c>
       <c r="B8" s="1">
         <f>1/B4*B7</f>
-        <v>0.16955017301038064</v>
+        <v>0.1692573402417962</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -21061,7 +21070,7 @@
       </c>
       <c r="B12">
         <f>COUNTIF(Data!D:D,"False")</f>
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -21070,7 +21079,7 @@
       </c>
       <c r="B13" s="1">
         <f>1/B4*B11</f>
-        <v>0.5017301038062284</v>
+        <v>0.50086355785837644</v>
       </c>
     </row>
   </sheetData>

</xml_diff>